<commit_message>
CT display and bug fixes
</commit_message>
<xml_diff>
--- a/AncillaryFiles/Wiggle_Summary_New.xlsx
+++ b/AncillaryFiles/Wiggle_Summary_New.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5762" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26762" uniqueCount="137">
   <si>
     <t>Subject</t>
   </si>
@@ -444,7 +444,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="153">
+  <borders count="433">
     <border>
       <left/>
       <right/>
@@ -604,11 +604,291 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="433">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -762,6 +1042,286 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="236" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="237" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="238" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="239" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="240" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="241" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="242" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="243" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="244" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="245" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="246" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="247" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="248" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="250" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="251" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,55 +1334,55 @@
   <dimension ref="A1:J71"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.64453125" customWidth="true"/>
-    <col min="2" max="2" width="10.37890625" customWidth="true"/>
-    <col min="3" max="3" width="11.64453125" customWidth="true"/>
-    <col min="4" max="4" width="14.1796875" customWidth="true"/>
-    <col min="5" max="5" width="17.578125" customWidth="true"/>
-    <col min="6" max="6" width="15.578125" customWidth="true"/>
-    <col min="7" max="7" width="17.11328125" customWidth="true"/>
-    <col min="8" max="8" width="15.11328125" customWidth="true"/>
-    <col min="9" max="9" width="14.84375" customWidth="true"/>
-    <col min="10" max="10" width="12.84375" customWidth="true"/>
+    <col min="1" max="1" width="11.28515625" customWidth="true"/>
+    <col min="2" max="2" width="10.5703125" customWidth="true"/>
+    <col min="3" max="3" width="12" customWidth="true"/>
+    <col min="4" max="4" width="15.7109375" customWidth="true"/>
+    <col min="5" max="5" width="19.5703125" customWidth="true"/>
+    <col min="6" max="6" width="17.28515625" customWidth="true"/>
+    <col min="7" max="7" width="19" customWidth="true"/>
+    <col min="8" max="8" width="16.7109375" customWidth="true"/>
+    <col min="9" max="9" width="16.5703125" customWidth="true"/>
+    <col min="10" max="10" width="14.28515625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="431" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151" t="s">
+      <c r="B1" s="431" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="431" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="151" t="s">
+      <c r="D1" s="431" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="151" t="s">
+      <c r="E1" s="431" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="151" t="s">
+      <c r="F1" s="431" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="151" t="s">
+      <c r="G1" s="431" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="151" t="s">
+      <c r="H1" s="431" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="151" t="s">
+      <c r="I1" s="431" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="151" t="s">
+      <c r="J1" s="431" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="431" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="431" t="s">
         <v>3</v>
       </c>
       <c r="C2">
@@ -851,10 +1411,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="431" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="431" t="s">
         <v>13</v>
       </c>
       <c r="C3">
@@ -883,10 +1443,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="431" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="431" t="s">
         <v>15</v>
       </c>
       <c r="C4">
@@ -915,10 +1475,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="151" t="s">
+      <c r="A5" s="431" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="431" t="s">
         <v>17</v>
       </c>
       <c r="C5">
@@ -947,10 +1507,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="151" t="s">
+      <c r="A6" s="431" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="151" t="s">
+      <c r="B6" s="431" t="s">
         <v>19</v>
       </c>
       <c r="C6">
@@ -979,10 +1539,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="431" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="431" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -1011,10 +1571,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="151" t="s">
+      <c r="A8" s="431" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="151" t="s">
+      <c r="B8" s="431" t="s">
         <v>23</v>
       </c>
       <c r="C8">
@@ -1043,10 +1603,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="151" t="s">
+      <c r="A9" s="431" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="151" t="s">
+      <c r="B9" s="431" t="s">
         <v>25</v>
       </c>
       <c r="C9">
@@ -1075,10 +1635,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="151" t="s">
+      <c r="A10" s="431" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="151" t="s">
+      <c r="B10" s="431" t="s">
         <v>27</v>
       </c>
       <c r="C10">
@@ -1107,10 +1667,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="151" t="s">
+      <c r="A11" s="431" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="151" t="s">
+      <c r="B11" s="431" t="s">
         <v>29</v>
       </c>
       <c r="C11">
@@ -1139,10 +1699,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="151" t="s">
+      <c r="A12" s="431" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="151" t="s">
+      <c r="B12" s="431" t="s">
         <v>31</v>
       </c>
       <c r="C12">
@@ -1171,10 +1731,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="431" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="151" t="s">
+      <c r="B13" s="431" t="s">
         <v>33</v>
       </c>
       <c r="C13">
@@ -1203,10 +1763,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="151" t="s">
+      <c r="A14" s="431" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="151" t="s">
+      <c r="B14" s="431" t="s">
         <v>35</v>
       </c>
       <c r="C14">
@@ -1235,10 +1795,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="151" t="s">
+      <c r="A15" s="431" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="151" t="s">
+      <c r="B15" s="431" t="s">
         <v>35</v>
       </c>
       <c r="C15">
@@ -1267,10 +1827,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="151" t="s">
+      <c r="A16" s="431" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="431" t="s">
         <v>38</v>
       </c>
       <c r="C16">
@@ -1299,10 +1859,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="151" t="s">
+      <c r="A17" s="431" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="431" t="s">
         <v>40</v>
       </c>
       <c r="C17">
@@ -1331,10 +1891,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="151" t="s">
+      <c r="A18" s="431" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="151" t="s">
+      <c r="B18" s="431" t="s">
         <v>40</v>
       </c>
       <c r="C18">
@@ -1363,10 +1923,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="151" t="s">
+      <c r="A19" s="431" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="431" t="s">
         <v>43</v>
       </c>
       <c r="C19">
@@ -1395,10 +1955,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="151" t="s">
+      <c r="A20" s="431" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="151" t="s">
+      <c r="B20" s="431" t="s">
         <v>45</v>
       </c>
       <c r="C20">
@@ -1427,10 +1987,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="151" t="s">
+      <c r="A21" s="431" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="151" t="s">
+      <c r="B21" s="431" t="s">
         <v>47</v>
       </c>
       <c r="C21">
@@ -1459,10 +2019,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="151" t="s">
+      <c r="A22" s="431" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="151" t="s">
+      <c r="B22" s="431" t="s">
         <v>49</v>
       </c>
       <c r="C22">
@@ -1491,10 +2051,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="151" t="s">
+      <c r="A23" s="431" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="151" t="s">
+      <c r="B23" s="431" t="s">
         <v>51</v>
       </c>
       <c r="C23">
@@ -1523,10 +2083,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="151" t="s">
+      <c r="A24" s="431" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="151" t="s">
+      <c r="B24" s="431" t="s">
         <v>53</v>
       </c>
       <c r="C24">
@@ -1555,10 +2115,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="151" t="s">
+      <c r="A25" s="431" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="151" t="s">
+      <c r="B25" s="431" t="s">
         <v>55</v>
       </c>
       <c r="C25">
@@ -1587,10 +2147,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="151" t="s">
+      <c r="A26" s="431" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="151" t="s">
+      <c r="B26" s="431" t="s">
         <v>57</v>
       </c>
       <c r="C26">
@@ -1619,10 +2179,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="151" t="s">
+      <c r="A27" s="431" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="151" t="s">
+      <c r="B27" s="431" t="s">
         <v>59</v>
       </c>
       <c r="C27">
@@ -1651,10 +2211,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="151" t="s">
+      <c r="A28" s="431" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="151" t="s">
+      <c r="B28" s="431" t="s">
         <v>61</v>
       </c>
       <c r="C28">
@@ -1683,10 +2243,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="151" t="s">
+      <c r="A29" s="431" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="151" t="s">
+      <c r="B29" s="431" t="s">
         <v>63</v>
       </c>
       <c r="C29">
@@ -1715,10 +2275,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="151" t="s">
+      <c r="A30" s="431" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="151" t="s">
+      <c r="B30" s="431" t="s">
         <v>65</v>
       </c>
       <c r="C30">
@@ -1747,10 +2307,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="151" t="s">
+      <c r="A31" s="431" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="151" t="s">
+      <c r="B31" s="431" t="s">
         <v>67</v>
       </c>
       <c r="C31">
@@ -1779,10 +2339,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="151" t="s">
+      <c r="A32" s="431" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="151" t="s">
+      <c r="B32" s="431" t="s">
         <v>69</v>
       </c>
       <c r="C32">
@@ -1811,10 +2371,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="151" t="s">
+      <c r="A33" s="431" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="151" t="s">
+      <c r="B33" s="431" t="s">
         <v>71</v>
       </c>
       <c r="C33">
@@ -1843,10 +2403,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="151" t="s">
+      <c r="A34" s="431" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="151" t="s">
+      <c r="B34" s="431" t="s">
         <v>73</v>
       </c>
       <c r="C34">
@@ -1875,10 +2435,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="151" t="s">
+      <c r="A35" s="431" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="151" t="s">
+      <c r="B35" s="431" t="s">
         <v>75</v>
       </c>
       <c r="C35">
@@ -1907,10 +2467,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="151" t="s">
+      <c r="A36" s="431" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="151" t="s">
+      <c r="B36" s="431" t="s">
         <v>75</v>
       </c>
       <c r="C36">
@@ -1939,10 +2499,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="151" t="s">
+      <c r="A37" s="431" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="151" t="s">
+      <c r="B37" s="431" t="s">
         <v>78</v>
       </c>
       <c r="C37">
@@ -1971,10 +2531,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="151" t="s">
+      <c r="A38" s="431" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="151" t="s">
+      <c r="B38" s="431" t="s">
         <v>80</v>
       </c>
       <c r="C38">
@@ -2003,10 +2563,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="151" t="s">
+      <c r="A39" s="431" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="151" t="s">
+      <c r="B39" s="431" t="s">
         <v>82</v>
       </c>
       <c r="C39">
@@ -2035,10 +2595,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="151" t="s">
+      <c r="A40" s="431" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="151" t="s">
+      <c r="B40" s="431" t="s">
         <v>84</v>
       </c>
       <c r="C40">
@@ -2067,10 +2627,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="151" t="s">
+      <c r="A41" s="431" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="151" t="s">
+      <c r="B41" s="431" t="s">
         <v>86</v>
       </c>
       <c r="C41">
@@ -2099,10 +2659,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="151" t="s">
+      <c r="A42" s="431" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="151" t="s">
+      <c r="B42" s="431" t="s">
         <v>88</v>
       </c>
       <c r="C42">
@@ -2131,10 +2691,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="151" t="s">
+      <c r="A43" s="431" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="151" t="s">
+      <c r="B43" s="431" t="s">
         <v>90</v>
       </c>
       <c r="C43">
@@ -2163,10 +2723,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="151" t="s">
+      <c r="A44" s="431" t="s">
         <v>91</v>
       </c>
-      <c r="B44" s="151" t="s">
+      <c r="B44" s="431" t="s">
         <v>90</v>
       </c>
       <c r="C44">
@@ -2195,10 +2755,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="151" t="s">
+      <c r="A45" s="431" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="151" t="s">
+      <c r="B45" s="431" t="s">
         <v>93</v>
       </c>
       <c r="C45">
@@ -2227,10 +2787,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="151" t="s">
+      <c r="A46" s="431" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="151" t="s">
+      <c r="B46" s="431" t="s">
         <v>95</v>
       </c>
       <c r="C46">
@@ -2259,10 +2819,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="151" t="s">
+      <c r="A47" s="431" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="151" t="s">
+      <c r="B47" s="431" t="s">
         <v>97</v>
       </c>
       <c r="C47">
@@ -2291,10 +2851,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="151" t="s">
+      <c r="A48" s="431" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="151" t="s">
+      <c r="B48" s="431" t="s">
         <v>97</v>
       </c>
       <c r="C48">
@@ -2323,10 +2883,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="151" t="s">
+      <c r="A49" s="431" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="151" t="s">
+      <c r="B49" s="431" t="s">
         <v>100</v>
       </c>
       <c r="C49">
@@ -2355,10 +2915,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="151" t="s">
+      <c r="A50" s="431" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="151" t="s">
+      <c r="B50" s="431" t="s">
         <v>100</v>
       </c>
       <c r="C50">
@@ -2387,10 +2947,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="151" t="s">
+      <c r="A51" s="431" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="151" t="s">
+      <c r="B51" s="431" t="s">
         <v>103</v>
       </c>
       <c r="C51">
@@ -2419,10 +2979,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="151" t="s">
+      <c r="A52" s="431" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="151" t="s">
+      <c r="B52" s="431" t="s">
         <v>105</v>
       </c>
       <c r="C52">
@@ -2451,10 +3011,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="151" t="s">
+      <c r="A53" s="431" t="s">
         <v>106</v>
       </c>
-      <c r="B53" s="151" t="s">
+      <c r="B53" s="431" t="s">
         <v>105</v>
       </c>
       <c r="C53">
@@ -2483,10 +3043,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="151" t="s">
+      <c r="A54" s="431" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="151" t="s">
+      <c r="B54" s="431" t="s">
         <v>108</v>
       </c>
       <c r="C54">
@@ -2515,10 +3075,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="151" t="s">
+      <c r="A55" s="431" t="s">
         <v>109</v>
       </c>
-      <c r="B55" s="151" t="s">
+      <c r="B55" s="431" t="s">
         <v>110</v>
       </c>
       <c r="C55">
@@ -2547,10 +3107,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="151" t="s">
+      <c r="A56" s="431" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="151" t="s">
+      <c r="B56" s="431" t="s">
         <v>112</v>
       </c>
       <c r="C56">
@@ -2579,10 +3139,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="151" t="s">
+      <c r="A57" s="431" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="151" t="s">
+      <c r="B57" s="431" t="s">
         <v>112</v>
       </c>
       <c r="C57">
@@ -2611,10 +3171,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="151" t="s">
+      <c r="A58" s="431" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="151" t="s">
+      <c r="B58" s="431" t="s">
         <v>115</v>
       </c>
       <c r="C58">
@@ -2643,10 +3203,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="151" t="s">
+      <c r="A59" s="431" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="151" t="s">
+      <c r="B59" s="431" t="s">
         <v>117</v>
       </c>
       <c r="C59">
@@ -2675,10 +3235,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="151" t="s">
+      <c r="A60" s="431" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="151" t="s">
+      <c r="B60" s="431" t="s">
         <v>117</v>
       </c>
       <c r="C60">
@@ -2707,10 +3267,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="151" t="s">
+      <c r="A61" s="431" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="151" t="s">
+      <c r="B61" s="431" t="s">
         <v>120</v>
       </c>
       <c r="C61">
@@ -2739,10 +3299,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="151" t="s">
+      <c r="A62" s="431" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="151" t="s">
+      <c r="B62" s="431" t="s">
         <v>122</v>
       </c>
       <c r="C62">
@@ -2771,10 +3331,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="151" t="s">
+      <c r="A63" s="431" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="151" t="s">
+      <c r="B63" s="431" t="s">
         <v>124</v>
       </c>
       <c r="C63">
@@ -2803,10 +3363,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="151" t="s">
+      <c r="A64" s="431" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="151" t="s">
+      <c r="B64" s="431" t="s">
         <v>124</v>
       </c>
       <c r="C64">
@@ -2835,10 +3395,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="151" t="s">
+      <c r="A65" s="431" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="151" t="s">
+      <c r="B65" s="431" t="s">
         <v>127</v>
       </c>
       <c r="C65">
@@ -2867,10 +3427,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="151" t="s">
+      <c r="A66" s="431" t="s">
         <v>128</v>
       </c>
-      <c r="B66" s="151" t="s">
+      <c r="B66" s="431" t="s">
         <v>129</v>
       </c>
       <c r="C66">
@@ -2899,10 +3459,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="151" t="s">
+      <c r="A67" s="431" t="s">
         <v>130</v>
       </c>
-      <c r="B67" s="151" t="s">
+      <c r="B67" s="431" t="s">
         <v>129</v>
       </c>
       <c r="C67">
@@ -2931,10 +3491,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="151" t="s">
+      <c r="A68" s="431" t="s">
         <v>131</v>
       </c>
-      <c r="B68" s="151" t="s">
+      <c r="B68" s="431" t="s">
         <v>132</v>
       </c>
       <c r="C68">
@@ -2963,10 +3523,10 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="151" t="s">
+      <c r="A69" s="431" t="s">
         <v>133</v>
       </c>
-      <c r="B69" s="151" t="s">
+      <c r="B69" s="431" t="s">
         <v>134</v>
       </c>
       <c r="C69">
@@ -2995,10 +3555,10 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="151" t="s">
+      <c r="A70" s="431" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="151" t="s">
+      <c r="B70" s="431" t="s">
         <v>3</v>
       </c>
       <c r="C70">
@@ -3027,10 +3587,10 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="151" t="s">
+      <c r="A71" s="431" t="s">
         <v>136</v>
       </c>
-      <c r="B71" s="151" t="s">
+      <c r="B71" s="431" t="s">
         <v>3</v>
       </c>
       <c r="C71">

</xml_diff>